<commit_message>
Add info managent database design.
</commit_message>
<xml_diff>
--- a/SohoWeb/database/Soho数据库设计.xlsx
+++ b/SohoWeb/database/Soho数据库设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="SohoCRM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="182">
   <si>
     <t>字段名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -691,6 +691,53 @@
   </si>
   <si>
     <t>日志内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmailAndSMSTemplates</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮件短信模板表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模板系统编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Templates</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>nvarchar(20)</t>
+  </si>
+  <si>
+    <t>nvarchar(MAX)</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模板内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email-Email模板；SMS-短信模板</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -780,7 +827,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -788,6 +835,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -798,12 +854,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1100,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:F14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1117,16 +1167,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="J1" t="s">
         <v>21</v>
       </c>
@@ -1367,16 +1417,16 @@
       <c r="F14" s="2"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
@@ -1602,16 +1652,222 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:F17"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:F33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C16 C18:C1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C16 C18:C32 C34:C1048576">
       <formula1>IsPK</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
@@ -1642,16 +1898,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="J1" t="s">
         <v>21</v>
       </c>
@@ -1758,16 +2014,16 @@
       <c r="F6" s="2"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
@@ -1826,10 +2082,10 @@
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>90</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1838,13 +2094,13 @@
       <c r="D12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1856,13 +2112,13 @@
       <c r="D13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1874,13 +2130,13 @@
       <c r="D14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1892,13 +2148,13 @@
       <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>95</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1910,13 +2166,13 @@
       <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>96</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1928,13 +2184,13 @@
       <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>97</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1946,13 +2202,13 @@
       <c r="D18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>98</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1964,13 +2220,13 @@
       <c r="D19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1982,13 +2238,13 @@
       <c r="D20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>100</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2000,13 +2256,13 @@
       <c r="D21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>101</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2018,13 +2274,13 @@
       <c r="D22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>102</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2036,22 +2292,22 @@
       <c r="D23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="4" t="s">
         <v>103</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4" t="s">
+      <c r="B25" s="6"/>
+      <c r="C25" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
@@ -2092,10 +2348,10 @@
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -2104,13 +2360,13 @@
       <c r="D28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2122,13 +2378,13 @@
       <c r="D29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -2140,13 +2396,13 @@
       <c r="D30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -2158,13 +2414,13 @@
       <c r="D31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="4" t="s">
         <v>109</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2176,13 +2432,13 @@
       <c r="D32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2194,13 +2450,13 @@
       <c r="D33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="4" t="s">
         <v>100</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -2212,13 +2468,13 @@
       <c r="D34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>101</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2230,13 +2486,13 @@
       <c r="D35" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="4" t="s">
         <v>102</v>
       </c>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -2248,7 +2504,7 @@
       <c r="D36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="4" t="s">
         <v>103</v>
       </c>
       <c r="F36" s="2"/>
@@ -2280,7 +2536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -2294,16 +2550,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="J1" t="s">
         <v>21</v>
       </c>
@@ -2368,7 +2624,7 @@
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>118</v>
       </c>
       <c r="F4" s="2"/>
@@ -2386,7 +2642,7 @@
       <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F5" s="2"/>
@@ -2404,7 +2660,7 @@
       <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>120</v>
       </c>
       <c r="F6" s="2"/>
@@ -2416,13 +2672,13 @@
       <c r="B7" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F7" s="2"/>
@@ -2524,16 +2780,16 @@
       <c r="F13" s="2"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
@@ -2574,10 +2830,10 @@
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>130</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -2586,13 +2842,13 @@
       <c r="D18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>131</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>124</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2604,13 +2860,13 @@
       <c r="D19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>132</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>125</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -2622,13 +2878,13 @@
       <c r="D20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>133</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>126</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2640,13 +2896,13 @@
       <c r="D21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>134</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2658,7 +2914,7 @@
       <c r="D22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F22" s="2"/>
@@ -2760,16 +3016,16 @@
       <c r="F28" s="2"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="6"/>
+      <c r="C30" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
@@ -2810,10 +3066,10 @@
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -2822,16 +3078,16 @@
       <c r="D33" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -2840,7 +3096,7 @@
       <c r="D34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>138</v>
       </c>
       <c r="F34" s="2"/>
@@ -2942,16 +3198,16 @@
       <c r="F40" s="2"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="4" t="s">
+      <c r="B42" s="6"/>
+      <c r="C42" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
@@ -2992,10 +3248,10 @@
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="4" t="s">
         <v>142</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -3004,16 +3260,16 @@
       <c r="D45" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="4" t="s">
         <v>143</v>
       </c>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -3022,7 +3278,7 @@
       <c r="D46" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F46" s="2"/>
@@ -3124,16 +3380,16 @@
       <c r="F52" s="2"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="4" t="s">
+      <c r="B54" s="6"/>
+      <c r="C54" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1" t="s">
@@ -3174,7 +3430,7 @@
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="4" t="s">
         <v>146</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -3186,13 +3442,13 @@
       <c r="D57" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -3204,13 +3460,13 @@
       <c r="D58" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -3222,7 +3478,7 @@
       <c r="D59" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F59" s="2"/>
@@ -3324,16 +3580,16 @@
       <c r="F65" s="2"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="4" t="s">
+      <c r="B67" s="6"/>
+      <c r="C67" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="1" t="s">
@@ -3374,10 +3630,10 @@
       <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C70" s="2" t="s">
@@ -3386,16 +3642,16 @@
       <c r="D70" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E70" s="6" t="s">
+      <c r="E70" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -3404,7 +3660,7 @@
       <c r="D71" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E71" s="4" t="s">
         <v>138</v>
       </c>
       <c r="F71" s="2"/>
@@ -3506,16 +3762,16 @@
       <c r="F77" s="2"/>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="3"/>
-      <c r="C79" s="4" t="s">
+      <c r="B79" s="6"/>
+      <c r="C79" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="1" t="s">
@@ -3556,10 +3812,10 @@
       <c r="F81" s="2"/>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C82" s="2" t="s">
@@ -3568,13 +3824,13 @@
       <c r="D82" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E82" s="6" t="s">
+      <c r="E82" s="4" t="s">
         <v>155</v>
       </c>
       <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="4" t="s">
         <v>153</v>
       </c>
       <c r="B83" s="2" t="s">
@@ -3586,13 +3842,13 @@
       <c r="D83" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E83" s="6" t="s">
+      <c r="E83" s="4" t="s">
         <v>156</v>
       </c>
       <c r="F83" s="2"/>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -3604,22 +3860,22 @@
       <c r="D84" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E84" s="6" t="s">
+      <c r="E84" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F84" s="2"/>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B86" s="3"/>
-      <c r="C86" s="4" t="s">
+      <c r="B86" s="6"/>
+      <c r="C86" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
@@ -3660,10 +3916,10 @@
       <c r="F88" s="2"/>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="6" t="s">
+      <c r="A89" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C89" s="2" t="s">
@@ -3672,13 +3928,13 @@
       <c r="D89" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E89" s="4" t="s">
         <v>164</v>
       </c>
       <c r="F89" s="2"/>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="6" t="s">
+      <c r="A90" s="4" t="s">
         <v>160</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -3690,13 +3946,13 @@
       <c r="D90" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E90" s="6" t="s">
+      <c r="E90" s="4" t="s">
         <v>165</v>
       </c>
       <c r="F90" s="2"/>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="6" t="s">
+      <c r="A91" s="4" t="s">
         <v>161</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -3708,13 +3964,13 @@
       <c r="D91" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E91" s="6" t="s">
+      <c r="E91" s="4" t="s">
         <v>166</v>
       </c>
       <c r="F91" s="2"/>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="4" t="s">
         <v>162</v>
       </c>
       <c r="B92" s="2" t="s">
@@ -3726,13 +3982,13 @@
       <c r="D92" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E92" s="6" t="s">
+      <c r="E92" s="4" t="s">
         <v>167</v>
       </c>
       <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="6" t="s">
+      <c r="A93" s="4" t="s">
         <v>163</v>
       </c>
       <c r="B93" s="2" t="s">
@@ -3744,7 +4000,7 @@
       <c r="D93" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E93" s="6" t="s">
+      <c r="E93" s="4" t="s">
         <v>168</v>
       </c>
       <c r="F93" s="2"/>
@@ -3799,6 +4055,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:F30"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="C79:F79"/>
     <mergeCell ref="A86:B86"/>
@@ -3809,12 +4071,6 @@
     <mergeCell ref="C54:F54"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="C67:F67"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:F30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">

</xml_diff>